<commit_message>
Rewrote the learning algorithm using numpy matrices, making the iterations computationally faster and the code cleaner
</commit_message>
<xml_diff>
--- a/bac.xlsx
+++ b/bac.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qaz11\Code\tensorflow_projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qaz11\Code\linear-regression-gradient-descent\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -497,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="R128" sqref="O97:R128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>